<commit_message>
Stefan Voievod, Domn al Tarii Moldovei
</commit_message>
<xml_diff>
--- a/data/best.xlsx
+++ b/data/best.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rpaproject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C50B9B8-FCAB-4786-B98F-334EA7A76B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ACF78B-62CF-4887-B8D1-8E49B1F18BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,10 +380,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3498</v>
+        <v>3298</v>
       </c>
       <c r="C2" s="1">
-        <v>44569.634722222225</v>
+        <v>44573.549305555556</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -391,10 +391,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1599</v>
+        <v>1399</v>
       </c>
       <c r="C3" s="1">
-        <v>44569.634027777778</v>
+        <v>44573.548611111109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bucuratu-m-am tare cand vazautu-mi-au ochii ale cerului minuni
</commit_message>
<xml_diff>
--- a/data/best.xlsx
+++ b/data/best.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rpaproject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ACF78B-62CF-4887-B8D1-8E49B1F18BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B2951-6B73-4F16-B79E-9A0A5EC79471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Code</t>
   </si>
@@ -36,10 +36,13 @@
     <t>Date</t>
   </si>
   <si>
+    <t xml:space="preserve">DL341015898541WP </t>
+  </si>
+  <si>
     <t>NH.Q8QEX.006</t>
   </si>
   <si>
-    <t xml:space="preserve">DL341015898541WP </t>
+    <t>G713IC-HX008</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,24 +380,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>3298</v>
       </c>
       <c r="C2" s="1">
-        <v>44573.549305555556</v>
+        <v>44573.595833333333</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1399</v>
       </c>
       <c r="C3" s="1">
-        <v>44573.548611111109</v>
+        <v>44573.595138888886</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44573.595138888886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>